<commit_message>
create BasePage and VyTrackDashboardPage.java and VyTrackLoginPage and wtite cods, but is have bug
</commit_message>
<xml_diff>
--- a/VyTrackQa2Users.xlsx
+++ b/VyTrackQa2Users.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Murodil/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ihork\IdeaProjects\CucumberProjectB24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{853B064B-C0EA-B344-8EC3-426B28EA3AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="2500" windowWidth="27240" windowHeight="16440" xr2:uid="{47319A83-4017-A548-AEBB-A2F2B1387863}"/>
+    <workbookView xWindow="3585" yWindow="2505" windowWidth="27240" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -108,12 +107,6 @@
     <t>storemanager52</t>
   </si>
   <si>
-    <t>Eddie</t>
-  </si>
-  <si>
-    <t>Rodriguez</t>
-  </si>
-  <si>
     <t>storemanager53</t>
   </si>
   <si>
@@ -190,12 +183,18 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Roma</t>
+  </si>
+  <si>
+    <t>Medhurst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -229,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -540,16 +539,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B45CC427-CF7F-3D44-80B5-6A431C042EC8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,10 +565,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -580,10 +582,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -597,10 +599,10 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -614,10 +616,10 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -631,10 +633,10 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -648,10 +650,10 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -665,10 +667,10 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -676,149 +678,149 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="D12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="s">
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="D13" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="D14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>42</v>
       </c>
-      <c r="D14" t="s">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="E14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="D15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add CLASSNOTES_DAY09_OFFICEHOURS_01.txt.txt and work with new mockaro class, updating BrowserUtils (add scroolDown method) and add manu new classes for mockaroo working
</commit_message>
<xml_diff>
--- a/VyTrackQa2Users.xlsx
+++ b/VyTrackQa2Users.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>username</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Turner</t>
   </si>
   <si>
-    <t>storemanager52</t>
-  </si>
-  <si>
     <t>storemanager53</t>
   </si>
   <si>
@@ -183,12 +180,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Roma</t>
-  </si>
-  <si>
-    <t>Medhurst</t>
   </si>
 </sst>
 </file>
@@ -540,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -565,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -582,7 +573,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,7 +590,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -616,7 +607,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -633,7 +624,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -650,7 +641,7 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -667,7 +658,7 @@
         <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,149 +669,132 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>